<commit_message>
Mise a vide certains test XML
</commit_message>
<xml_diff>
--- a/data/P1_EX1 - Definition du Référentiel - Ayoub Benhadou - Kevin Durand.xlsx
+++ b/data/P1_EX1 - Definition du Référentiel - Ayoub Benhadou - Kevin Durand.xlsx
@@ -1,14 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\__M2_MIAGE__\ID\Mediateur_M2APP\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28770" windowHeight="12270" activeTab="2"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Source 1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Source 2" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Source 3" sheetId="3" r:id="rId5"/>
+    <sheet name="Source 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Source 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Source 3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -257,16 +265,8 @@
 (IF S1.T_Excel.Statut == "etudiant")</t>
   </si>
   <si>
-    <t xml:space="preserve">Valeur(M.Etudiant.Provenance) == Valeur(S2.Etudiant.Provenance)
-</t>
-  </si>
-  <si>
     <t>Etudiant.FormationPrecedente
 Type = Varchar(45)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valeur(M.Etudiant.FormationPrecedente) == Valeur(S2.Etudiant.FormationPrecedente)
-</t>
   </si>
   <si>
     <t xml:space="preserve">Etudiant.PaysFormationPrecedente
@@ -278,13 +278,17 @@
       <rPr>
         <b/>
         <i/>
+        <sz val="10"/>
         <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Note :</t>
     </r>
     <r>
       <rPr>
         <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> year-from-date est une fonction XQuery qui retourne l'annee 
 d'une date xs:date
@@ -332,13 +336,17 @@
       <rPr>
         <b/>
         <i/>
+        <sz val="10"/>
         <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Note :</t>
     </r>
     <r>
       <rPr>
         <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> SYSDATE correspondant à la date d'aujourd'hui en SQL Oracle. 
 Nous avons appliqué un masque 'yyyy' pour ne recuperer que l'année de la date.</t>
@@ -808,46 +816,74 @@
   <si>
     <t>Valeur(M.Enseigne.Annee) == Valeur (S2.Enseigne.Annee)</t>
   </si>
+  <si>
+    <t>M.Etudiant.Provenance.'France' == ValeurS2.Etudiant.Provenance.'fr'
+M.Etudiant.Provenance.'Italie' == ValeurS2.Etudiant.Provenance.'it'
+M.Etudiant.Provenance.'Allemagne' == ValeurS2.Etudiant.Provenance.'de'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.Etudiant.FormationPrecedente.'France' == ValeurS2.Etudiant.FormationPrecedente.'fr'
+M.Etudiant.FormationPrecedente.'Italie' == ValeurS2.Etudiant.FormationPrecedente.'it'
+M.Etudiant.FormationPrecedente.'Allemagne' == ValeurS2.Etudiant.FormationPrecedente.'de'
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="7.0"/>
+      <sz val="7"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -862,9 +898,27 @@
         <bgColor rgb="FFB7B7B7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -878,27 +932,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -908,101 +969,369 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf quotePrefix="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.14"/>
-    <col customWidth="1" min="2" max="2" width="30.29"/>
-    <col customWidth="1" min="3" max="3" width="74.14"/>
+    <col min="1" max="1" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="107.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,18 +1345,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1038,7 +1367,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1049,7 +1378,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -1060,7 +1389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1071,7 +1400,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" ht="49.5" customHeight="1">
+    <row r="7" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
@@ -1082,7 +1411,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>40</v>
       </c>
@@ -1093,7 +1422,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
@@ -1104,7 +1433,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -1115,214 +1444,214 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12">
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="B13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14">
+    </row>
+    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="C14" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-    </row>
-    <row r="17">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="D17" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="4" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="5" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C19" s="4" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C20" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:4" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B25" s="17" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="16" t="s">
+      <c r="C25" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="16" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="B26" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="17"/>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="16"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:4" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B30" s="17" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="16" t="s">
+      <c r="C30" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="B30" s="16" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1330,26 +1659,30 @@
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A27:C27"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.57"/>
-    <col customWidth="1" min="2" max="2" width="39.43"/>
-    <col customWidth="1" min="3" max="3" width="82.71"/>
+    <col min="1" max="1" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1363,7 +1696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1374,7 +1707,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1385,7 +1718,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1396,281 +1729,281 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5" s="22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="B7" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="B9" s="20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="C9" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="D9" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10">
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12">
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13">
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="B15" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-    </row>
-    <row r="17">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="5" t="s">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C19" s="4" t="s">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="C20" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="s">
-        <v>156</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" s="5" t="s">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>168</v>
-      </c>
       <c r="C25" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="17"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="16"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" s="5" t="s">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="31">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1678,26 +2011,29 @@
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A27:C27"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.57"/>
-    <col customWidth="1" min="2" max="2" width="60.43"/>
-    <col customWidth="1" min="3" max="3" width="96.71"/>
+    <col min="1" max="1" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1719,7 +2055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1730,7 +2066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1741,7 +2077,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -1752,7 +2088,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1763,7 +2099,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
@@ -1774,7 +2110,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -1785,99 +2121,99 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" ht="40.5" customHeight="1">
+    <row r="9" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="D9" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="4" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="B14" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="B15" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="B17" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18">
+    </row>
+    <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>12</v>
@@ -1886,135 +2222,135 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="5" t="s">
+    <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22">
+    </row>
+    <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B25" s="5" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="17"/>
+    <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="16"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C29" s="5" t="s">
+    <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="5" t="s">
+      <c r="B30" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C30" s="5" t="s">
+    </row>
+    <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>180</v>
-      </c>
       <c r="C31" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2022,6 +2358,6 @@
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A27:C27"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>